<commit_message>
adding function for replacing values
</commit_message>
<xml_diff>
--- a/scripts/label_mapping.xlsx
+++ b/scripts/label_mapping.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21050" windowHeight="10470" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21045" windowHeight="10470"/>
   </bookViews>
   <sheets>
     <sheet name="operations" sheetId="6" r:id="rId1"/>
-    <sheet name="income_change" sheetId="3" r:id="rId2"/>
-    <sheet name="crop_prod_diff_main" sheetId="2" r:id="rId3"/>
-    <sheet name="columns_renaming" sheetId="1" r:id="rId4"/>
-    <sheet name="DifficultyRaisingAnimals" sheetId="4" r:id="rId5"/>
-    <sheet name="AllAnswerOptions" sheetId="5" r:id="rId6"/>
-    <sheet name="correct_values" sheetId="7" r:id="rId7"/>
+    <sheet name="columns_renaming" sheetId="1" r:id="rId2"/>
+    <sheet name="values_replacing" sheetId="7" r:id="rId3"/>
+    <sheet name="crop_planted_area_comp" sheetId="8" r:id="rId4"/>
+    <sheet name="income_change" sheetId="3" r:id="rId5"/>
+    <sheet name="crop_prod_diff_main" sheetId="2" r:id="rId6"/>
+    <sheet name="DifficultyRaisingAnimals" sheetId="4" r:id="rId7"/>
+    <sheet name="AllAnswerOptions" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">AllAnswerOptions!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">crop_prod_diff_main!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">AllAnswerOptions!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">crop_prod_diff_main!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="175">
   <si>
     <t>AnswerOptions</t>
   </si>
@@ -505,12 +506,6 @@
     <t>columns_renaming</t>
   </si>
   <si>
-    <t>column_renaming</t>
-  </si>
-  <si>
-    <t>column_name</t>
-  </si>
-  <si>
     <t>new_value</t>
   </si>
   <si>
@@ -545,13 +540,37 @@
   </si>
   <si>
     <t>crop_planted_area_comp</t>
+  </si>
+  <si>
+    <t>column</t>
+  </si>
+  <si>
+    <t>Difficulty to access fertilizers or pesticides</t>
+  </si>
+  <si>
+    <t>Difficulty to access seeds</t>
+  </si>
+  <si>
+    <t>Dryspell/drought</t>
+  </si>
+  <si>
+    <t>Heavy rains/floods</t>
+  </si>
+  <si>
+    <t>Lower irrigation than usual</t>
+  </si>
+  <si>
+    <t>Access to land restricted by containment measures</t>
+  </si>
+  <si>
+    <t>values_replacing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -586,6 +605,13 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -714,7 +740,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -786,6 +812,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1066,21 +1093,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>148</v>
       </c>
@@ -1091,12 +1118,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>146</v>
       </c>
@@ -1104,20 +1131,28 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>149</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>152</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>154</v>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1128,95 +1163,226 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7265625" customWidth="1"/>
+    <col min="1" max="1" width="51.5703125" customWidth="1"/>
+    <col min="2" max="2" width="72.42578125" customWidth="1"/>
+    <col min="3" max="3" width="72" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="12">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="12">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4" s="12">
+    <row r="2" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5" s="12">
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B6" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" s="12">
+    <row r="3" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="B8" s="12">
+      <c r="B3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+    <row r="4" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+      <c r="B18" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="12">
-        <v>9</v>
+      <c r="B19" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1226,19 +1392,582 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>152</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>152</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>152</v>
+      </c>
+      <c r="B27" t="s">
+        <v>173</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>152</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>152</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37" s="27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="12">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="12">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.7265625" customWidth="1"/>
-    <col min="2" max="2" width="30.26953125" customWidth="1"/>
+    <col min="1" max="1" width="55.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1246,7 +1975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>57</v>
       </c>
@@ -1254,7 +1983,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>58</v>
       </c>
@@ -1262,7 +1991,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>59</v>
       </c>
@@ -1270,7 +1999,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>60</v>
       </c>
@@ -1278,7 +2007,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>61</v>
       </c>
@@ -1286,7 +2015,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>62</v>
       </c>
@@ -1294,7 +2023,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>63</v>
       </c>
@@ -1302,7 +2031,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
@@ -1310,7 +2039,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>64</v>
       </c>
@@ -1318,7 +2047,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>65</v>
       </c>
@@ -1326,7 +2055,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>67</v>
       </c>
@@ -1334,7 +2063,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>69</v>
       </c>
@@ -1342,7 +2071,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>71</v>
       </c>
@@ -1350,7 +2079,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>73</v>
       </c>
@@ -1358,7 +2087,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>75</v>
       </c>
@@ -1366,7 +2095,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>77</v>
       </c>
@@ -1374,7 +2103,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>79</v>
       </c>
@@ -1382,7 +2111,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>81</v>
       </c>
@@ -1390,7 +2119,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>83</v>
       </c>
@@ -1398,7 +2127,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>85</v>
       </c>
@@ -1406,7 +2135,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>87</v>
       </c>
@@ -1414,7 +2143,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>89</v>
       </c>
@@ -1422,7 +2151,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>91</v>
       </c>
@@ -1430,7 +2159,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>48</v>
       </c>
@@ -1438,7 +2167,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>94</v>
       </c>
@@ -1446,7 +2175,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>96</v>
       </c>
@@ -1454,7 +2183,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>98</v>
       </c>
@@ -1462,7 +2191,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>100</v>
       </c>
@@ -1470,7 +2199,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>102</v>
       </c>
@@ -1478,7 +2207,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>104</v>
       </c>
@@ -1486,7 +2215,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>106</v>
       </c>
@@ -1504,228 +2233,57 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.54296875" customWidth="1"/>
-    <col min="2" max="2" width="72.453125" customWidth="1"/>
-    <col min="3" max="3" width="72" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="4">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="8" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="4">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1733,65 +2291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="4">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C63"/>
   <sheetViews>
@@ -1799,14 +2299,14 @@
       <selection activeCell="A42" sqref="A42:A59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.1796875" style="21" customWidth="1"/>
-    <col min="2" max="2" width="35.54296875" customWidth="1"/>
-    <col min="3" max="3" width="36.26953125" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>118</v>
       </c>
@@ -1817,7 +2317,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>121</v>
       </c>
@@ -1828,7 +2328,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23"/>
       <c r="B3" s="14" t="s">
         <v>58</v>
@@ -1837,7 +2337,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="14" t="s">
         <v>122</v>
@@ -1846,7 +2346,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
       <c r="B5" s="14" t="s">
         <v>123</v>
@@ -1855,7 +2355,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
       <c r="B6" s="14" t="s">
         <v>124</v>
@@ -1864,7 +2364,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="23"/>
       <c r="B7" s="14" t="s">
         <v>125</v>
@@ -1873,7 +2373,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
       <c r="B8" s="14" t="s">
         <v>122</v>
@@ -1882,7 +2382,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="14" t="s">
         <v>126</v>
@@ -1891,7 +2391,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="14" t="s">
         <v>127</v>
@@ -1900,7 +2400,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>128</v>
       </c>
@@ -1911,7 +2411,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="14" t="s">
         <v>110</v>
@@ -1920,7 +2420,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
       <c r="B13" s="14" t="s">
         <v>111</v>
@@ -1929,7 +2429,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
       <c r="B14" s="14" t="s">
         <v>112</v>
@@ -1938,7 +2438,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
       <c r="B15" s="14" t="s">
         <v>113</v>
@@ -1947,7 +2447,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23"/>
       <c r="B16" s="14" t="s">
         <v>114</v>
@@ -1956,7 +2456,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
       <c r="B17" s="14" t="s">
         <v>115</v>
@@ -1965,7 +2465,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
       <c r="B18" s="14" t="s">
         <v>51</v>
@@ -1974,7 +2474,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="23"/>
       <c r="B19" s="14" t="s">
         <v>54</v>
@@ -1983,7 +2483,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23"/>
       <c r="B20" s="14" t="s">
         <v>65</v>
@@ -1992,7 +2492,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23"/>
       <c r="B21" s="14" t="s">
         <v>67</v>
@@ -2001,7 +2501,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="23"/>
       <c r="B22" s="14" t="s">
         <v>122</v>
@@ -2010,7 +2510,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
       <c r="B23" s="14" t="s">
         <v>122</v>
@@ -2019,7 +2519,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
       <c r="B24" s="14" t="s">
         <v>122</v>
@@ -2028,7 +2528,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="23"/>
       <c r="B25" s="14" t="s">
         <v>122</v>
@@ -2037,7 +2537,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="23"/>
       <c r="B26" s="14" t="s">
         <v>122</v>
@@ -2046,7 +2546,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
       <c r="B27" s="14" t="s">
         <v>79</v>
@@ -2055,7 +2555,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23"/>
       <c r="B28" s="14" t="s">
         <v>81</v>
@@ -2064,7 +2564,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="23"/>
       <c r="B29" s="14" t="s">
         <v>131</v>
@@ -2073,7 +2573,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="23"/>
       <c r="B30" s="14" t="s">
         <v>85</v>
@@ -2082,7 +2582,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="23"/>
       <c r="B31" s="14" t="s">
         <v>87</v>
@@ -2091,7 +2591,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="23"/>
       <c r="B32" s="14" t="s">
         <v>89</v>
@@ -2100,7 +2600,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="23"/>
       <c r="B33" s="14" t="s">
         <v>91</v>
@@ -2109,7 +2609,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="23"/>
       <c r="B34" s="14" t="s">
         <v>48</v>
@@ -2118,7 +2618,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="23"/>
       <c r="B35" s="14" t="s">
         <v>51</v>
@@ -2127,7 +2627,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="23"/>
       <c r="B36" s="15" t="s">
         <v>54</v>
@@ -2136,7 +2636,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="23"/>
       <c r="B37" s="17" t="s">
         <v>98</v>
@@ -2145,7 +2645,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="23"/>
       <c r="B38" s="14" t="s">
         <v>100</v>
@@ -2154,7 +2654,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="23"/>
       <c r="B39" s="14" t="s">
         <v>102</v>
@@ -2163,7 +2663,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="23"/>
       <c r="B40" s="14" t="s">
         <v>104</v>
@@ -2172,7 +2672,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="25"/>
       <c r="B41" s="14" t="s">
         <v>106</v>
@@ -2181,7 +2681,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
         <v>132</v>
       </c>
@@ -2192,7 +2692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="23"/>
       <c r="B43" s="14" t="s">
         <v>6</v>
@@ -2201,7 +2701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="23"/>
       <c r="B44" s="14" t="s">
         <v>9</v>
@@ -2210,7 +2710,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="23"/>
       <c r="B45" s="14" t="s">
         <v>12</v>
@@ -2219,7 +2719,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="23"/>
       <c r="B46" s="14" t="s">
         <v>15</v>
@@ -2228,7 +2728,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="23"/>
       <c r="B47" s="14" t="s">
         <v>18</v>
@@ -2237,7 +2737,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="23"/>
       <c r="B48" s="14" t="s">
         <v>21</v>
@@ -2246,7 +2746,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="23"/>
       <c r="B49" s="14" t="s">
         <v>24</v>
@@ -2255,7 +2755,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="23"/>
       <c r="B50" s="14" t="s">
         <v>27</v>
@@ -2264,7 +2764,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="23"/>
       <c r="B51" s="14" t="s">
         <v>30</v>
@@ -2273,7 +2773,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="23"/>
       <c r="B52" s="14" t="s">
         <v>33</v>
@@ -2282,7 +2782,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="23"/>
       <c r="B53" s="14" t="s">
         <v>36</v>
@@ -2291,7 +2791,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="23"/>
       <c r="B54" s="14" t="s">
         <v>39</v>
@@ -2300,7 +2800,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="23"/>
       <c r="B55" s="14" t="s">
         <v>42</v>
@@ -2309,7 +2809,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="23"/>
       <c r="B56" s="14" t="s">
         <v>45</v>
@@ -2318,7 +2818,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="23"/>
       <c r="B57" s="14" t="s">
         <v>48</v>
@@ -2327,7 +2827,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="23"/>
       <c r="B58" s="14" t="s">
         <v>51</v>
@@ -2336,7 +2836,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="23"/>
       <c r="B59" s="19" t="s">
         <v>54</v>
@@ -2345,7 +2845,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="26" t="s">
         <v>134</v>
       </c>
@@ -2356,7 +2856,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="26"/>
       <c r="B61" s="18" t="s">
         <v>117</v>
@@ -2365,7 +2865,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="26"/>
       <c r="B62" s="18" t="s">
         <v>51</v>
@@ -2374,7 +2874,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="26"/>
       <c r="B63" s="18" t="s">
         <v>54</v>
@@ -2399,122 +2899,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.90625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA0901C00BE8754680E1F02E394963D6" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21f7e0e2f49adfcb4ebf93b6942ecc8c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="651ac188-b77a-445d-b0b3-bedb0cff8e72" xmlns:ns3="4efa6d18-7e22-4963-b4bf-16e1a76dd523" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="676eb4c27537306e2855e8473b9e904a" ns2:_="" ns3:_="">
     <xsd:import namespace="651ac188-b77a-445d-b0b3-bedb0cff8e72"/>
@@ -2719,22 +3119,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BABAF42C-6384-4A26-A083-BECCC293D6BA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="651ac188-b77a-445d-b0b3-bedb0cff8e72"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4efa6d18-7e22-4963-b4bf-16e1a76dd523"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAD8E2E4-34C3-4CD1-9C6F-4832C7D2E6F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6783C02B-356E-412D-BFDB-C04FB81AE2EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2751,29 +3161,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAD8E2E4-34C3-4CD1-9C6F-4832C7D2E6F1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BABAF42C-6384-4A26-A083-BECCC293D6BA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="651ac188-b77a-445d-b0b3-bedb0cff8e72"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4efa6d18-7e22-4963-b4bf-16e1a76dd523"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>